<commit_message>
Run success create customer
</commit_message>
<xml_diff>
--- a/bin/testdata/TestData.xlsx
+++ b/bin/testdata/TestData.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Create New Account" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="35">
   <si>
     <t>https://portal.4te.vn/assets/img/logo_gas.jpg</t>
   </si>
@@ -42,19 +43,88 @@
     <t>currentImportPrice</t>
   </si>
   <si>
-    <t>manufacture</t>
-  </si>
-  <si>
     <t>Xám</t>
   </si>
   <si>
     <t>30/12/2020</t>
   </si>
   <si>
-    <t>5efc371a503fe9208cef0ffc</t>
-  </si>
-  <si>
-    <t>TEST1108001</t>
+    <t>email</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>Quận 9</t>
+  </si>
+  <si>
+    <t>Nhóm thực tế</t>
+  </si>
+  <si>
+    <t>Quận 1</t>
+  </si>
+  <si>
+    <t>Nhóm không tính</t>
+  </si>
+  <si>
+    <t>TEST1608001</t>
+  </si>
+  <si>
+    <t>TEST1608002</t>
+  </si>
+  <si>
+    <t>TEST1608003</t>
+  </si>
+  <si>
+    <t>TEST1608004</t>
+  </si>
+  <si>
+    <t>TEST1608005</t>
+  </si>
+  <si>
+    <t>TEST1608006</t>
+  </si>
+  <si>
+    <t>TEST1608007</t>
+  </si>
+  <si>
+    <t>TEST1608008</t>
+  </si>
+  <si>
+    <t>TEST1608009</t>
+  </si>
+  <si>
+    <t>TEST1608010</t>
+  </si>
+  <si>
+    <t>nhahangf@gmail.com</t>
+  </si>
+  <si>
+    <t>toanhaf@gmail.com</t>
+  </si>
+  <si>
+    <t>Nhà hàng F</t>
+  </si>
+  <si>
+    <t>Tòa nhà F</t>
+  </si>
+  <si>
+    <t>NH0013</t>
+  </si>
+  <si>
+    <t>NH0014</t>
+  </si>
+  <si>
+    <t>TN007</t>
   </si>
 </sst>
 </file>
@@ -118,7 +188,7 @@
       <name val="Roboto, sans-serif"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -131,8 +201,14 @@
         <bgColor rgb="FF0070C0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -140,12 +216,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -155,6 +246,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -428,7 +522,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -438,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -471,22 +565,20 @@
       <c r="F1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="E2">
         <v>693.6</v>
@@ -494,22 +586,20 @@
       <c r="F2" s="5">
         <v>556020</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="G2" s="8"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="E3">
         <v>693.6</v>
@@ -517,22 +607,20 @@
       <c r="F3" s="5">
         <v>556020</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="E4">
         <v>693.6</v>
@@ -540,22 +628,20 @@
       <c r="F4" s="5">
         <v>556020</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="G4" s="8"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="E5">
         <v>693.6</v>
@@ -563,22 +649,20 @@
       <c r="F5" s="5">
         <v>556020</v>
       </c>
-      <c r="G5" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="E6">
         <v>693.6</v>
@@ -586,22 +670,20 @@
       <c r="F6" s="5">
         <v>556020</v>
       </c>
-      <c r="G6" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="E7">
         <v>693.6</v>
@@ -609,22 +691,20 @@
       <c r="F7" s="5">
         <v>556020</v>
       </c>
-      <c r="G7" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="E8">
         <v>693.6</v>
@@ -632,22 +712,20 @@
       <c r="F8" s="5">
         <v>556020</v>
       </c>
-      <c r="G8" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="G8" s="8"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="E9">
         <v>693.6</v>
@@ -655,22 +733,20 @@
       <c r="F9" s="5">
         <v>556020</v>
       </c>
-      <c r="G9" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="G9" s="8"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="E10">
         <v>693.6</v>
@@ -678,22 +754,20 @@
       <c r="F10" s="5">
         <v>556020</v>
       </c>
-      <c r="G10" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="G10" s="8"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="E11">
         <v>693.6</v>
@@ -701,9 +775,7 @@
       <c r="F11" s="5">
         <v>556020</v>
       </c>
-      <c r="G11" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="G11" s="8"/>
     </row>
     <row r="12" spans="1:7">
       <c r="B12" s="7"/>
@@ -1065,4 +1137,101 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="31" style="5" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="16" style="5" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="5" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update project, add new function
</commit_message>
<xml_diff>
--- a/bin/testdata/TestData.xlsx
+++ b/bin/testdata/TestData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
   <si>
     <t>color</t>
   </si>
@@ -55,15 +55,6 @@
     <t>Nhóm không tính</t>
   </si>
   <si>
-    <t>TEST1608001</t>
-  </si>
-  <si>
-    <t>TEST1608002</t>
-  </si>
-  <si>
-    <t>TEST1608003</t>
-  </si>
-  <si>
     <t>nhahangf@gmail.com</t>
   </si>
   <si>
@@ -106,9 +97,6 @@
     <t>Compact</t>
   </si>
   <si>
-    <t>1 van</t>
-  </si>
-  <si>
     <t>13.9</t>
   </si>
   <si>
@@ -137,6 +125,21 @@
   </si>
   <si>
     <t>VT</t>
+  </si>
+  <si>
+    <t>verificationDate</t>
+  </si>
+  <si>
+    <t>1 Van</t>
+  </si>
+  <si>
+    <t>TEST1608004</t>
+  </si>
+  <si>
+    <t>TEST1608005</t>
+  </si>
+  <si>
+    <t>TEST1608006</t>
   </si>
 </sst>
 </file>
@@ -213,7 +216,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -222,6 +225,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -538,13 +542,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>7</v>
@@ -555,13 +559,13 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>9</v>
@@ -572,13 +576,13 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>7</v>
@@ -600,10 +604,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -612,89 +616,101 @@
     <col min="2" max="2" width="19.85546875" style="5" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" style="5" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" style="5" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="5"/>
+    <col min="5" max="6" width="16.42578125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>32</v>
       </c>
+      <c r="D2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="8">
+        <v>44072</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="7" t="s">
+    <row r="3" spans="1:7">
+      <c r="A3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="8">
+        <v>44075</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="7" t="s">
+      <c r="E4" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="7" t="s">
+      <c r="F4" s="8">
+        <v>44078</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix function create cylinder
</commit_message>
<xml_diff>
--- a/bin/testdata/TestData.xlsx
+++ b/bin/testdata/TestData.xlsx
@@ -4,13 +4,16 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13470" windowHeight="5475" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Create New Account" sheetId="2" r:id="rId1"/>
     <sheet name="Create Cylinder" sheetId="3" r:id="rId2"/>
+    <sheet name="CreateWithExistCode" sheetId="4" r:id="rId3"/>
+    <sheet name="CreateAccountWithExistCode" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <oleSize ref="A1:F16"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="52">
   <si>
     <t>color</t>
   </si>
@@ -55,27 +58,6 @@
     <t>Nhóm không tính</t>
   </si>
   <si>
-    <t>nhahangf@gmail.com</t>
-  </si>
-  <si>
-    <t>toanhaf@gmail.com</t>
-  </si>
-  <si>
-    <t>Nhà hàng F</t>
-  </si>
-  <si>
-    <t>Tòa nhà F</t>
-  </si>
-  <si>
-    <t>NH0013</t>
-  </si>
-  <si>
-    <t>NH0014</t>
-  </si>
-  <si>
-    <t>TN007</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
@@ -136,10 +118,67 @@
     <t>TEST1608004</t>
   </si>
   <si>
-    <t>TEST1608005</t>
-  </si>
-  <si>
-    <t>TEST1608006</t>
+    <t>TEST1908001</t>
+  </si>
+  <si>
+    <t>TEST1908002</t>
+  </si>
+  <si>
+    <t>TEST1908003</t>
+  </si>
+  <si>
+    <t>Đại lý phân phối 1</t>
+  </si>
+  <si>
+    <t>Đại lý phân phối 2</t>
+  </si>
+  <si>
+    <t>Đại lý phân phối 3</t>
+  </si>
+  <si>
+    <t>DLPP180801</t>
+  </si>
+  <si>
+    <t>dailyphanphoi180801@gmail.com</t>
+  </si>
+  <si>
+    <t>DLPP180802</t>
+  </si>
+  <si>
+    <t>DLPP180803</t>
+  </si>
+  <si>
+    <t>childId</t>
+  </si>
+  <si>
+    <t>childName</t>
+  </si>
+  <si>
+    <t>childAddress</t>
+  </si>
+  <si>
+    <t>CDLPP180801</t>
+  </si>
+  <si>
+    <t>CDLPP180802</t>
+  </si>
+  <si>
+    <t>CDLPP180803</t>
+  </si>
+  <si>
+    <t>Chi nhánh DLPP 18/08 01</t>
+  </si>
+  <si>
+    <t>Bình Dương</t>
+  </si>
+  <si>
+    <t>Chi nhánh DLPP 18/08 02</t>
+  </si>
+  <si>
+    <t>Chi nhánh DLPP 18/08 03</t>
+  </si>
+  <si>
+    <t>Đồng Nai</t>
   </si>
 </sst>
 </file>
@@ -499,7 +538,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -507,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C17" sqref="C16:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -520,10 +559,13 @@
     <col min="3" max="3" width="16" style="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="6" width="14.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -539,16 +581,25 @@
       <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>7</v>
@@ -556,16 +607,25 @@
       <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="4" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>9</v>
@@ -573,32 +633,49 @@
       <c r="E3" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>8</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A3:A4" r:id="rId2" display="dailyphanphoi180801@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -606,8 +683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -626,95 +703,244 @@
         <v>4</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F2" s="8">
         <v>44072</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="7" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F3" s="8">
         <v>44075</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="7" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F4" s="8">
         <v>44078</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="8">
+        <v>44072</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="30.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add function export cylinder
</commit_message>
<xml_diff>
--- a/bin/testdata/TestData.xlsx
+++ b/bin/testdata/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13470" windowHeight="5475" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13470" windowHeight="5220"/>
   </bookViews>
   <sheets>
     <sheet name="Create New Account" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="47">
   <si>
     <t>color</t>
   </si>
@@ -52,12 +52,6 @@
     <t>Nhóm thực tế</t>
   </si>
   <si>
-    <t>Quận 1</t>
-  </si>
-  <si>
-    <t>Nhóm không tính</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
@@ -130,24 +124,12 @@
     <t>Đại lý phân phối 1</t>
   </si>
   <si>
-    <t>Đại lý phân phối 2</t>
-  </si>
-  <si>
-    <t>Đại lý phân phối 3</t>
-  </si>
-  <si>
     <t>DLPP180801</t>
   </si>
   <si>
     <t>dailyphanphoi180801@gmail.com</t>
   </si>
   <si>
-    <t>DLPP180802</t>
-  </si>
-  <si>
-    <t>DLPP180803</t>
-  </si>
-  <si>
     <t>childId</t>
   </si>
   <si>
@@ -160,9 +142,6 @@
     <t>CDLPP180801</t>
   </si>
   <si>
-    <t>CDLPP180802</t>
-  </si>
-  <si>
     <t>CDLPP180803</t>
   </si>
   <si>
@@ -172,20 +151,26 @@
     <t>Bình Dương</t>
   </si>
   <si>
-    <t>Chi nhánh DLPP 18/08 02</t>
-  </si>
-  <si>
     <t>Chi nhánh DLPP 18/08 03</t>
   </si>
   <si>
     <t>Đồng Nai</t>
+  </si>
+  <si>
+    <t>DLPP180804</t>
+  </si>
+  <si>
+    <t>dailyphanphoi180805@gmail.com</t>
+  </si>
+  <si>
+    <t>Đại lý phân phối 5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,6 +196,12 @@
       <sz val="11"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -260,11 +251,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -538,7 +529,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -546,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C16:C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -582,24 +573,24 @@
         <v>6</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="4" t="s">
-        <v>38</v>
+      <c r="A2" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>7</v>
@@ -608,74 +599,21 @@
         <v>8</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3:A4" r:id="rId2" display="dailyphanphoi180801@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -689,105 +627,105 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="5" customWidth="1"/>
-    <col min="5" max="6" width="16.42578125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" style="5" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="13.140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="4" customWidth="1"/>
+    <col min="5" max="6" width="16.42578125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="6" t="s">
+      <c r="C2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="7">
+        <v>44072</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" s="6" t="s">
+      <c r="C3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="7">
+        <v>44075</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="7" t="s">
+    <row r="4" spans="1:7">
+      <c r="A4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="7" t="s">
+      <c r="D4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="8">
-        <v>44072</v>
-      </c>
-      <c r="G2" s="7" t="s">
+      <c r="F4" s="7">
+        <v>44078</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="8">
-        <v>44075</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="8">
-        <v>44078</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -815,49 +753,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="7" t="s">
+      <c r="C2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="8">
+      <c r="F2" s="7">
         <v>44072</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>22</v>
+      <c r="G2" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -869,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -902,24 +840,24 @@
         <v>6</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="4" t="s">
-        <v>38</v>
+      <c r="A2" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>7</v>
@@ -928,13 +866,13 @@
         <v>8</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -942,5 +880,6 @@
     <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix all function, add import cylinder
</commit_message>
<xml_diff>
--- a/bin/testdata/TestData.xlsx
+++ b/bin/testdata/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13470" windowHeight="5220"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13545" windowHeight="5475"/>
   </bookViews>
   <sheets>
     <sheet name="Create New Account" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
   <si>
     <t>color</t>
   </si>
@@ -112,15 +112,6 @@
     <t>TEST1608004</t>
   </si>
   <si>
-    <t>TEST1908001</t>
-  </si>
-  <si>
-    <t>TEST1908002</t>
-  </si>
-  <si>
-    <t>TEST1908003</t>
-  </si>
-  <si>
     <t>Đại lý phân phối 1</t>
   </si>
   <si>
@@ -142,28 +133,52 @@
     <t>CDLPP180801</t>
   </si>
   <si>
-    <t>CDLPP180803</t>
-  </si>
-  <si>
     <t>Chi nhánh DLPP 18/08 01</t>
   </si>
   <si>
     <t>Bình Dương</t>
   </si>
   <si>
-    <t>Chi nhánh DLPP 18/08 03</t>
-  </si>
-  <si>
     <t>Đồng Nai</t>
   </si>
   <si>
-    <t>DLPP180804</t>
-  </si>
-  <si>
-    <t>dailyphanphoi180805@gmail.com</t>
-  </si>
-  <si>
-    <t>Đại lý phân phối 5</t>
+    <t>TEST2208001</t>
+  </si>
+  <si>
+    <t>TEST2208002</t>
+  </si>
+  <si>
+    <t>TEST2208003</t>
+  </si>
+  <si>
+    <t>dailyphanphoi180806@gmail.com</t>
+  </si>
+  <si>
+    <t>Đại lý phân phối 6</t>
+  </si>
+  <si>
+    <t>DLPP180806</t>
+  </si>
+  <si>
+    <t>CDLPP180806</t>
+  </si>
+  <si>
+    <t>Chi nhánh DLPP 18/08 06</t>
+  </si>
+  <si>
+    <t>Chi nhánh DLPP 18/08 08</t>
+  </si>
+  <si>
+    <t>CDLPP180808</t>
+  </si>
+  <si>
+    <t>DLPP180808</t>
+  </si>
+  <si>
+    <t>Đại lý phân phối 8</t>
+  </si>
+  <si>
+    <t>dailyphanphoi180808@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -246,7 +261,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -256,6 +271,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -529,7 +545,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -537,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -573,21 +589,21 @@
         <v>6</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="8" t="s">
-        <v>45</v>
+      <c r="A2" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>44</v>
@@ -599,21 +615,48 @@
         <v>8</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -622,7 +665,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -661,7 +704,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="6" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>11</v>
@@ -684,7 +727,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="6" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>12</v>
@@ -707,7 +750,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="6" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>13</v>
@@ -840,24 +883,24 @@
         <v>6</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>7</v>
@@ -866,13 +909,13 @@
         <v>8</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
separate login and create user
</commit_message>
<xml_diff>
--- a/bin/testdata/TestData.xlsx
+++ b/bin/testdata/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13545" windowHeight="5295" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="12225" windowHeight="4590"/>
   </bookViews>
   <sheets>
     <sheet name="Create New Account" sheetId="2" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="CreateAccountWithExistCode" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:H16"/>
+  <oleSize ref="A1:E13"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -142,43 +142,43 @@
     <t>Đồng Nai</t>
   </si>
   <si>
-    <t>dailyphanphoi250801</t>
-  </si>
-  <si>
-    <t>dailyphanphoi250802</t>
-  </si>
-  <si>
-    <t>Đại lý phân phối 250801</t>
-  </si>
-  <si>
-    <t>Đại lý phân phối 250802</t>
-  </si>
-  <si>
-    <t>DLPP250801</t>
-  </si>
-  <si>
-    <t>DLPP250802</t>
-  </si>
-  <si>
-    <t>CDLPP250801</t>
-  </si>
-  <si>
-    <t>CDLPP250802</t>
-  </si>
-  <si>
-    <t>Chi nhánh DLPP 250801</t>
-  </si>
-  <si>
-    <t>Chi nhánh DLPP 250802</t>
-  </si>
-  <si>
-    <t>TEST2308019</t>
-  </si>
-  <si>
-    <t>TEST2308020</t>
-  </si>
-  <si>
-    <t>TEST2308021</t>
+    <t>dailyphanphoi240803</t>
+  </si>
+  <si>
+    <t>Đại lý phân phối 240803</t>
+  </si>
+  <si>
+    <t>DLPP240803</t>
+  </si>
+  <si>
+    <t>CDLPP240803</t>
+  </si>
+  <si>
+    <t>Chi nhánh DLPP 240803</t>
+  </si>
+  <si>
+    <t>dailyphanphoi240804</t>
+  </si>
+  <si>
+    <t>Đại lý phân phối 240804</t>
+  </si>
+  <si>
+    <t>DLPP240804</t>
+  </si>
+  <si>
+    <t>CDLPP240804</t>
+  </si>
+  <si>
+    <t>Chi nhánh DLPP 240804</t>
+  </si>
+  <si>
+    <t>TEST2408001</t>
+  </si>
+  <si>
+    <t>TEST2408002</t>
+  </si>
+  <si>
+    <t>TEST2408003</t>
   </si>
 </sst>
 </file>
@@ -544,7 +544,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -554,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -602,10 +602,10 @@
         <v>39</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>43</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>7</v>
@@ -614,10 +614,10 @@
         <v>8</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>38</v>
@@ -625,13 +625,13 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="8" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>7</v>
@@ -640,7 +640,7 @@
         <v>8</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>48</v>
@@ -651,11 +651,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="dailyphanphoi240801@gmail.com"/>
-    <hyperlink ref="A3" r:id="rId2" display="dailyphanphoi240801@gmail.com"/>
+    <hyperlink ref="A2:A3" r:id="rId1" display="dailyphanphoi240801@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -663,7 +662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>